<commit_message>
Added one test case and found bug
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87AA106-E15B-496D-B0E2-5220C8992BA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFB973F-A921-4478-B5B8-0C95F7B2A864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="66">
   <si>
     <t>Bug Log</t>
   </si>
@@ -219,6 +219,15 @@
   </si>
   <si>
     <t>Casper &amp; Bao Xian</t>
+  </si>
+  <si>
+    <t>Authenticate (web service)</t>
+  </si>
+  <si>
+    <t>Wrong username does not give expected output</t>
+  </si>
+  <si>
+    <t>Unresolved</t>
   </si>
 </sst>
 </file>
@@ -477,6 +486,12 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -487,27 +502,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none"/>
@@ -610,6 +609,16 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFF4CCCC"/>
           <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1004,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H999"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="91" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="91" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1022,16 +1031,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.4">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.4">
       <c r="A2" s="22" t="s">
@@ -1079,7 +1088,7 @@
         <f t="shared" ref="F3:F199" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="40">
         <f>SUM(F3:F21)</f>
         <v>97</v>
       </c>
@@ -1108,7 +1117,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G4" s="38"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.4">
@@ -1131,7 +1140,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="38"/>
+      <c r="G5" s="40"/>
       <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.4">
@@ -1154,7 +1163,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G6" s="38"/>
+      <c r="G6" s="40"/>
       <c r="H6" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.4">
@@ -1177,7 +1186,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G7" s="38"/>
+      <c r="G7" s="40"/>
       <c r="H7" s="24"/>
     </row>
     <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -1200,7 +1209,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G8" s="38"/>
+      <c r="G8" s="40"/>
       <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.4">
@@ -1223,7 +1232,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G9" s="38"/>
+      <c r="G9" s="40"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="1:8" ht="14.4" x14ac:dyDescent="0.4">
@@ -1246,7 +1255,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G10" s="38"/>
+      <c r="G10" s="40"/>
       <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -1269,7 +1278,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G11" s="38"/>
+      <c r="G11" s="40"/>
       <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -1292,7 +1301,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G12" s="38"/>
+      <c r="G12" s="40"/>
       <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:8" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -1315,7 +1324,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G13" s="38"/>
+      <c r="G13" s="40"/>
       <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -1337,7 +1346,7 @@
       <c r="F14" s="20">
         <v>1</v>
       </c>
-      <c r="G14" s="38"/>
+      <c r="G14" s="40"/>
       <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -1359,7 +1368,7 @@
       <c r="F15" s="20">
         <v>5</v>
       </c>
-      <c r="G15" s="38"/>
+      <c r="G15" s="40"/>
       <c r="H15" s="24"/>
     </row>
     <row r="16" spans="1:8" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -1381,7 +1390,7 @@
       <c r="F16" s="20">
         <v>1</v>
       </c>
-      <c r="G16" s="38"/>
+      <c r="G16" s="40"/>
       <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" ht="14.4" x14ac:dyDescent="0.4">
@@ -1403,7 +1412,7 @@
       <c r="F17" s="20">
         <v>5</v>
       </c>
-      <c r="G17" s="38"/>
+      <c r="G17" s="40"/>
       <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -1425,7 +1434,7 @@
       <c r="F18" s="20">
         <v>5</v>
       </c>
-      <c r="G18" s="38"/>
+      <c r="G18" s="40"/>
       <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -1447,7 +1456,7 @@
       <c r="F19" s="20">
         <v>10</v>
       </c>
-      <c r="G19" s="38"/>
+      <c r="G19" s="40"/>
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:8" ht="14.4" x14ac:dyDescent="0.55000000000000004">
@@ -1469,7 +1478,7 @@
       <c r="F20" s="20">
         <v>5</v>
       </c>
-      <c r="G20" s="38"/>
+      <c r="G20" s="40"/>
       <c r="H20" s="24"/>
     </row>
     <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.4">
@@ -1491,7 +1500,7 @@
       <c r="F21" s="20">
         <v>5</v>
       </c>
-      <c r="G21" s="38"/>
+      <c r="G21" s="40"/>
       <c r="H21" s="24"/>
     </row>
     <row r="22" spans="1:8" ht="14.4" x14ac:dyDescent="0.4">
@@ -1535,13 +1544,28 @@
         <f>IF($E23="Critical", 10, IF($E23="High",5, IF($E23="Low",1,"")))</f>
         <v>10</v>
       </c>
-      <c r="H23" s="41" t="s">
+      <c r="H23" s="37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="20">
         <v>22</v>
+      </c>
+      <c r="B24" s="21">
+        <v>2</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="21">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="14.4" x14ac:dyDescent="0.4">
@@ -6651,7 +6675,7 @@
     <mergeCell ref="G3:G21"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6668,8 +6692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -6686,16 +6710,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
@@ -7296,7 +7320,7 @@
       <c r="D23" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="38" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="19">
@@ -7313,11 +7337,21 @@
       <c r="A24" s="9">
         <v>14</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14"/>
+      <c r="B24" s="9">
+        <v>3</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="19">
+        <v>43748</v>
+      </c>
       <c r="G24" s="14"/>
       <c r="H24" s="13"/>
     </row>
@@ -7329,7 +7363,7 @@
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
-      <c r="E25" s="13"/>
+      <c r="E25" s="38"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="13"/>
@@ -7342,7 +7376,7 @@
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="13"/>
+      <c r="E26" s="38"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="13"/>
@@ -7355,7 +7389,7 @@
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
-      <c r="E27" s="13"/>
+      <c r="E27" s="38"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="13"/>
@@ -7368,7 +7402,7 @@
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
-      <c r="E28" s="13"/>
+      <c r="E28" s="38"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="13"/>
@@ -7378,7 +7412,7 @@
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
-      <c r="E29" s="13"/>
+      <c r="E29" s="38"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="13"/>
@@ -7388,7 +7422,7 @@
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
-      <c r="E30" s="13"/>
+      <c r="E30" s="38"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="13"/>
@@ -7398,7 +7432,7 @@
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="15"/>
-      <c r="E31" s="13"/>
+      <c r="E31" s="38"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
       <c r="H31" s="13"/>
@@ -7408,7 +7442,7 @@
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="10"/>
-      <c r="E32" s="13"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="13"/>
@@ -7418,7 +7452,7 @@
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="10"/>
-      <c r="E33" s="13"/>
+      <c r="E33" s="38"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="13"/>
@@ -7428,7 +7462,7 @@
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="10"/>
-      <c r="E34" s="13"/>
+      <c r="E34" s="38"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
       <c r="H34" s="13"/>
@@ -7438,7 +7472,7 @@
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="15"/>
-      <c r="E35" s="13"/>
+      <c r="E35" s="38"/>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
       <c r="H35" s="13"/>
@@ -7448,7 +7482,7 @@
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="10"/>
-      <c r="E36" s="13"/>
+      <c r="E36" s="38"/>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
       <c r="H36" s="13"/>
@@ -7458,7 +7492,7 @@
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="10"/>
-      <c r="E37" s="13"/>
+      <c r="E37" s="38"/>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
       <c r="H37" s="13"/>
@@ -7468,7 +7502,7 @@
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
-      <c r="E38" s="13"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
       <c r="H38" s="13"/>
@@ -17098,82 +17132,82 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="cellIs" dxfId="15" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="cellIs" dxfId="14" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="23" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="containsBlanks" dxfId="13" priority="24">
+    <cfRule type="containsBlanks" dxfId="12" priority="24">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+  <conditionalFormatting sqref="E23:E38">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+  <conditionalFormatting sqref="E23:E38">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="containsBlanks" dxfId="10" priority="12">
+  <conditionalFormatting sqref="E23:E38">
+    <cfRule type="containsBlanks" dxfId="9" priority="12">
       <formula>LEN(TRIM(E23))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsBlanks" dxfId="7" priority="9">
+    <cfRule type="containsBlanks" dxfId="6" priority="9">
       <formula>LEN(TRIM(E12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="containsBlanks" dxfId="4" priority="6">
+    <cfRule type="containsBlanks" dxfId="3" priority="6">
       <formula>LEN(TRIM(E21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="containsBlanks" dxfId="1" priority="3">
+    <cfRule type="containsBlanks" dxfId="0" priority="3">
       <formula>LEN(TRIM(E22))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E3:E23" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="E3:E38" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Unresolved,Resolved"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add to bug log
successful bid wit bid amount with more than 2 decimal places
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\project-g4t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD95DA8B-BED9-483E-88CE-36C182B233A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39EC239-A1AF-4EC5-A974-16F56294ADC5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="75">
   <si>
     <t>Bug Log</t>
   </si>
@@ -1043,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="91" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A19" zoomScale="91" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6647,8 +6647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32:D33"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7416,7 +7416,9 @@
       <c r="C29" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="17"/>
+      <c r="D29" s="17" t="s">
+        <v>72</v>
+      </c>
       <c r="E29" s="38" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
add delete bid bug
unable to delete bid
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\project-g4t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39EC239-A1AF-4EC5-A974-16F56294ADC5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7133677D-60C1-4BB8-8FBA-DC2020AC7B09}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="76">
   <si>
     <t>Bug Log</t>
   </si>
@@ -256,6 +256,9 @@
   <si>
     <t>Delete Bid</t>
   </si>
+  <si>
+    <t xml:space="preserve">Failed to delete bid. Successful deletion message shows even before user selects section to delete. </t>
+  </si>
 </sst>
 </file>
 
@@ -380,7 +383,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -403,11 +406,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -532,6 +550,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,7 +1065,7 @@
   <dimension ref="A1:H999"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="91" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1732,14 +1753,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
         <v>29</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="F31" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B31" s="26">
+        <v>2</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="39">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -6648,7 +6680,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C30" sqref="C30:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7428,7 +7460,7 @@
       <c r="G29" s="14"/>
       <c r="H29" s="13"/>
     </row>
-    <row r="30" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>28</v>
       </c>
@@ -7438,9 +7470,15 @@
       <c r="C30" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="14"/>
+      <c r="D30" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>73</v>
+      </c>
       <c r="G30" s="14"/>
       <c r="H30" s="13"/>
     </row>

</xml_diff>

<commit_message>
resolved bug for delete bid
updating
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\project-g4t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7133677D-60C1-4BB8-8FBA-DC2020AC7B09}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF30280-BD80-4EAB-9C6F-CD745E6EC9B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="76">
   <si>
     <t>Bug Log</t>
   </si>
@@ -540,6 +540,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,9 +553,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H999"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="91" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A23" zoomScale="91" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1082,16 +1082,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -1139,7 +1139,7 @@
         <f t="shared" ref="F3:F199" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G3" s="41">
+      <c r="G3" s="42">
         <v>0</v>
       </c>
       <c r="H3" s="24" t="str">
@@ -1167,7 +1167,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G4" s="41"/>
+      <c r="G4" s="42"/>
       <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -1190,7 +1190,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="41"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.25">
@@ -1213,7 +1213,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G6" s="41"/>
+      <c r="G6" s="42"/>
       <c r="H6" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -1236,7 +1236,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G7" s="41"/>
+      <c r="G7" s="42"/>
       <c r="H7" s="24"/>
     </row>
     <row r="8" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -1259,7 +1259,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G8" s="41"/>
+      <c r="G8" s="42"/>
       <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -1282,7 +1282,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G9" s="41"/>
+      <c r="G9" s="42"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -1305,7 +1305,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G10" s="41"/>
+      <c r="G10" s="42"/>
       <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -1328,7 +1328,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G11" s="41"/>
+      <c r="G11" s="42"/>
       <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -1351,7 +1351,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G12" s="41"/>
+      <c r="G12" s="42"/>
       <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -1374,7 +1374,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G13" s="41"/>
+      <c r="G13" s="42"/>
       <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -1396,7 +1396,7 @@
       <c r="F14" s="39">
         <v>1</v>
       </c>
-      <c r="G14" s="41"/>
+      <c r="G14" s="42"/>
       <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -1418,7 +1418,7 @@
       <c r="F15" s="39">
         <v>5</v>
       </c>
-      <c r="G15" s="41"/>
+      <c r="G15" s="42"/>
       <c r="H15" s="24"/>
     </row>
     <row r="16" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -1440,7 +1440,7 @@
       <c r="F16" s="39">
         <v>1</v>
       </c>
-      <c r="G16" s="41"/>
+      <c r="G16" s="42"/>
       <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -1462,7 +1462,7 @@
       <c r="F17" s="39">
         <v>5</v>
       </c>
-      <c r="G17" s="41"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -1484,7 +1484,7 @@
       <c r="F18" s="39">
         <v>5</v>
       </c>
-      <c r="G18" s="41"/>
+      <c r="G18" s="42"/>
       <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -1506,7 +1506,7 @@
       <c r="F19" s="39">
         <v>10</v>
       </c>
-      <c r="G19" s="41"/>
+      <c r="G19" s="42"/>
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -1528,7 +1528,7 @@
       <c r="F20" s="39">
         <v>5</v>
       </c>
-      <c r="G20" s="41"/>
+      <c r="G20" s="42"/>
       <c r="H20" s="24"/>
     </row>
     <row r="21" spans="1:8" ht="29" x14ac:dyDescent="0.25">
@@ -1550,7 +1550,7 @@
       <c r="F21" s="39">
         <v>5</v>
       </c>
-      <c r="G21" s="41"/>
+      <c r="G21" s="42"/>
       <c r="H21" s="24"/>
     </row>
     <row r="22" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
@@ -1572,7 +1572,7 @@
       <c r="F22" s="39">
         <v>5</v>
       </c>
-      <c r="G22" s="41">
+      <c r="G22" s="42">
         <v>0</v>
       </c>
       <c r="H22" s="24"/>
@@ -1597,7 +1597,7 @@
         <f>IF($E23="Critical", 10, IF($E23="High",5, IF($E23="Low",1,"")))</f>
         <v>10</v>
       </c>
-      <c r="G23" s="41"/>
+      <c r="G23" s="42"/>
       <c r="H23" s="37" t="s">
         <v>23</v>
       </c>
@@ -1621,7 +1621,7 @@
       <c r="F24" s="39">
         <v>1</v>
       </c>
-      <c r="G24" s="41">
+      <c r="G24" s="42">
         <v>0</v>
       </c>
     </row>
@@ -1644,7 +1644,7 @@
       <c r="F25" s="39">
         <v>5</v>
       </c>
-      <c r="G25" s="41"/>
+      <c r="G25" s="42"/>
     </row>
     <row r="26" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
@@ -1665,7 +1665,7 @@
       <c r="F26" s="39">
         <v>1</v>
       </c>
-      <c r="G26" s="41"/>
+      <c r="G26" s="42"/>
     </row>
     <row r="27" spans="1:8" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A27" s="20">
@@ -1686,7 +1686,7 @@
       <c r="F27" s="39">
         <v>5</v>
       </c>
-      <c r="G27" s="41"/>
+      <c r="G27" s="42"/>
       <c r="H27" s="37" t="s">
         <v>23</v>
       </c>
@@ -1763,7 +1763,7 @@
       <c r="C31" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="44" t="s">
+      <c r="D31" s="40" t="s">
         <v>75</v>
       </c>
       <c r="E31" s="39" t="s">
@@ -6679,8 +6679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:D30"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6697,16 +6697,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
     </row>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -7470,17 +7470,21 @@
       <c r="C30" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="44" t="s">
+      <c r="D30" s="40" t="s">
         <v>75</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="F30" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G30" s="14"/>
-      <c r="H30" s="13"/>
+      <c r="G30" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>

</xml_diff>

<commit_message>
Include bugs found when doing testing
Bugs on update bid function.
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ong Yan Ning\Desktop\SMU\Academic\Year 2 Term 1\IS212 - Software Project Management\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ong Yan Ning\Documents\GitHub\project-g4t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B28BE53-C9AE-47CC-A056-38C2CE923969}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449ED0F2-AB9F-4A14-95A2-063021424450}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="79">
   <si>
     <t>Bug Log</t>
   </si>
@@ -257,6 +257,9 @@
   <si>
     <t>Errors when updating bid - non numeric value encountered</t>
   </si>
+  <si>
+    <t>Errors when updating bid - uncaught argument count error due to too few arguments to function BidDAO.</t>
+  </si>
 </sst>
 </file>
 
@@ -408,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -523,6 +526,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -533,7 +539,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1089,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="91" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="91" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1107,16 +1122,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -1164,7 +1179,7 @@
         <f t="shared" ref="F3:F199" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G3" s="41">
+      <c r="G3" s="42">
         <v>0</v>
       </c>
       <c r="H3" s="24" t="str">
@@ -1192,7 +1207,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G4" s="41"/>
+      <c r="G4" s="42"/>
       <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1215,7 +1230,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="41"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -1238,7 +1253,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G6" s="41"/>
+      <c r="G6" s="42"/>
       <c r="H6" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1261,7 +1276,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G7" s="41"/>
+      <c r="G7" s="42"/>
       <c r="H7" s="24"/>
     </row>
     <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1284,7 +1299,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G8" s="41"/>
+      <c r="G8" s="42"/>
       <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1307,7 +1322,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G9" s="41"/>
+      <c r="G9" s="42"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1330,7 +1345,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G10" s="41"/>
+      <c r="G10" s="42"/>
       <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1353,7 +1368,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G11" s="41"/>
+      <c r="G11" s="42"/>
       <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1376,7 +1391,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G12" s="41"/>
+      <c r="G12" s="42"/>
       <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1399,7 +1414,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G13" s="41"/>
+      <c r="G13" s="42"/>
       <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1421,7 +1436,7 @@
       <c r="F14" s="39">
         <v>1</v>
       </c>
-      <c r="G14" s="41"/>
+      <c r="G14" s="42"/>
       <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1443,7 +1458,7 @@
       <c r="F15" s="39">
         <v>5</v>
       </c>
-      <c r="G15" s="41"/>
+      <c r="G15" s="42"/>
       <c r="H15" s="24"/>
     </row>
     <row r="16" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1465,7 +1480,7 @@
       <c r="F16" s="39">
         <v>1</v>
       </c>
-      <c r="G16" s="41"/>
+      <c r="G16" s="42"/>
       <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1487,7 +1502,7 @@
       <c r="F17" s="39">
         <v>5</v>
       </c>
-      <c r="G17" s="41"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1509,7 +1524,7 @@
       <c r="F18" s="39">
         <v>5</v>
       </c>
-      <c r="G18" s="41"/>
+      <c r="G18" s="42"/>
       <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1531,7 +1546,7 @@
       <c r="F19" s="39">
         <v>10</v>
       </c>
-      <c r="G19" s="41"/>
+      <c r="G19" s="42"/>
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1553,7 +1568,7 @@
       <c r="F20" s="39">
         <v>5</v>
       </c>
-      <c r="G20" s="41"/>
+      <c r="G20" s="42"/>
       <c r="H20" s="24"/>
     </row>
     <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -1575,7 +1590,7 @@
       <c r="F21" s="39">
         <v>5</v>
       </c>
-      <c r="G21" s="41"/>
+      <c r="G21" s="42"/>
       <c r="H21" s="24"/>
     </row>
     <row r="22" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1597,7 +1612,7 @@
       <c r="F22" s="39">
         <v>5</v>
       </c>
-      <c r="G22" s="41">
+      <c r="G22" s="42">
         <v>0</v>
       </c>
       <c r="H22" s="24"/>
@@ -1622,7 +1637,7 @@
         <f>IF($E23="Critical", 10, IF($E23="High",5, IF($E23="Low",1,"")))</f>
         <v>10</v>
       </c>
-      <c r="G23" s="41"/>
+      <c r="G23" s="42"/>
       <c r="H23" s="37" t="s">
         <v>23</v>
       </c>
@@ -1646,7 +1661,7 @@
       <c r="F24" s="39">
         <v>1</v>
       </c>
-      <c r="G24" s="41">
+      <c r="G24" s="42">
         <v>0</v>
       </c>
     </row>
@@ -1669,7 +1684,7 @@
       <c r="F25" s="39">
         <v>5</v>
       </c>
-      <c r="G25" s="41"/>
+      <c r="G25" s="42"/>
     </row>
     <row r="26" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
@@ -1690,7 +1705,7 @@
       <c r="F26" s="39">
         <v>1</v>
       </c>
-      <c r="G26" s="41"/>
+      <c r="G26" s="42"/>
     </row>
     <row r="27" spans="1:8" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A27" s="20">
@@ -1711,7 +1726,7 @@
       <c r="F27" s="39">
         <v>5</v>
       </c>
-      <c r="G27" s="41"/>
+      <c r="G27" s="42"/>
       <c r="H27" s="37" t="s">
         <v>23</v>
       </c>
@@ -1788,7 +1803,7 @@
       <c r="C31" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="44" t="s">
+      <c r="D31" s="40" t="s">
         <v>75</v>
       </c>
       <c r="E31" s="39" t="s">
@@ -1841,14 +1856,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A34" s="20">
         <v>33</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="F34" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B34" s="26">
+        <v>2</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="39">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
@@ -6726,8 +6752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6744,16 +6770,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
     </row>
     <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -7348,7 +7374,7 @@
       <c r="B23" s="9">
         <v>2</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="45" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="17" t="s">
@@ -7367,17 +7393,17 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>14</v>
       </c>
       <c r="B24" s="9">
         <v>2</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="48" t="s">
         <v>64</v>
       </c>
       <c r="E24" s="38" t="s">
@@ -7401,7 +7427,7 @@
       <c r="B25" s="39">
         <v>2</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="46" t="s">
         <v>66</v>
       </c>
       <c r="D25" s="24" t="s">
@@ -7424,7 +7450,7 @@
       <c r="B26" s="39">
         <v>2</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="46" t="s">
         <v>66</v>
       </c>
       <c r="D26" s="24" t="s">
@@ -7447,7 +7473,7 @@
       <c r="B27" s="9">
         <v>2</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="45" t="s">
         <v>66</v>
       </c>
       <c r="D27" s="17" t="s">
@@ -7470,7 +7496,7 @@
       <c r="B28" s="9">
         <v>2</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="45" t="s">
         <v>56</v>
       </c>
       <c r="D28" s="17" t="s">
@@ -7492,7 +7518,7 @@
       <c r="B29" s="9">
         <v>2</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="45" t="s">
         <v>56</v>
       </c>
       <c r="D29" s="17" t="s">
@@ -7514,10 +7540,10 @@
       <c r="B30" s="9">
         <v>2</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="44" t="s">
+      <c r="D30" s="40" t="s">
         <v>75</v>
       </c>
       <c r="E30" s="38" t="s">
@@ -7540,20 +7566,24 @@
       <c r="B31" s="9">
         <v>2</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="45" t="s">
         <v>42</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>76</v>
       </c>
       <c r="E31" s="38" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="F31" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G31" s="14"/>
-      <c r="H31" s="13"/>
+      <c r="G31" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
@@ -7562,7 +7592,7 @@
       <c r="B32" s="9">
         <v>2</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="45" t="s">
         <v>56</v>
       </c>
       <c r="D32" s="17" t="s">
@@ -7577,13 +7607,25 @@
       <c r="G32" s="14"/>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="14"/>
+    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="9">
+        <v>31</v>
+      </c>
+      <c r="B33" s="9">
+        <v>2</v>
+      </c>
+      <c r="C33" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>73</v>
+      </c>
       <c r="G33" s="14"/>
       <c r="H33" s="13"/>
     </row>

</xml_diff>

<commit_message>
Bootstrap bugs when testing
Bugs found when testing bootstrap function (manual)
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ong Yan Ning\Documents\GitHub\project-g4t4\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ong Yan Ning\Desktop\SMU\Academic\Year 2 Term 1\IS212 - Software Project Management\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449ED0F2-AB9F-4A14-95A2-063021424450}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F1C9D8-9964-44CF-96AA-E3065D68E69C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="80">
   <si>
     <t>Bug Log</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>Errors when updating bid - uncaught argument count error due to too few arguments to function BidDAO.</t>
+  </si>
+  <si>
+    <t>Integrity constraint violation - cannot delete or update a parent row</t>
   </si>
 </sst>
 </file>
@@ -529,16 +532,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -551,6 +544,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1104,7 +1107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="91" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="91" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
@@ -1122,16 +1125,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -1179,7 +1182,7 @@
         <f t="shared" ref="F3:F199" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G3" s="42">
+      <c r="G3" s="46">
         <v>0</v>
       </c>
       <c r="H3" s="24" t="str">
@@ -1207,7 +1210,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G4" s="42"/>
+      <c r="G4" s="46"/>
       <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1230,7 +1233,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="42"/>
+      <c r="G5" s="46"/>
       <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -1253,7 +1256,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G6" s="42"/>
+      <c r="G6" s="46"/>
       <c r="H6" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1276,7 +1279,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G7" s="42"/>
+      <c r="G7" s="46"/>
       <c r="H7" s="24"/>
     </row>
     <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1299,7 +1302,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G8" s="42"/>
+      <c r="G8" s="46"/>
       <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1322,7 +1325,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G9" s="42"/>
+      <c r="G9" s="46"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1345,7 +1348,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G10" s="42"/>
+      <c r="G10" s="46"/>
       <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1368,7 +1371,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G11" s="42"/>
+      <c r="G11" s="46"/>
       <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1391,7 +1394,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G12" s="42"/>
+      <c r="G12" s="46"/>
       <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1414,7 +1417,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G13" s="42"/>
+      <c r="G13" s="46"/>
       <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1436,7 +1439,7 @@
       <c r="F14" s="39">
         <v>1</v>
       </c>
-      <c r="G14" s="42"/>
+      <c r="G14" s="46"/>
       <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1458,7 +1461,7 @@
       <c r="F15" s="39">
         <v>5</v>
       </c>
-      <c r="G15" s="42"/>
+      <c r="G15" s="46"/>
       <c r="H15" s="24"/>
     </row>
     <row r="16" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1480,7 +1483,7 @@
       <c r="F16" s="39">
         <v>1</v>
       </c>
-      <c r="G16" s="42"/>
+      <c r="G16" s="46"/>
       <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1502,7 +1505,7 @@
       <c r="F17" s="39">
         <v>5</v>
       </c>
-      <c r="G17" s="42"/>
+      <c r="G17" s="46"/>
       <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1524,7 +1527,7 @@
       <c r="F18" s="39">
         <v>5</v>
       </c>
-      <c r="G18" s="42"/>
+      <c r="G18" s="46"/>
       <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1546,7 +1549,7 @@
       <c r="F19" s="39">
         <v>10</v>
       </c>
-      <c r="G19" s="42"/>
+      <c r="G19" s="46"/>
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1568,7 +1571,7 @@
       <c r="F20" s="39">
         <v>5</v>
       </c>
-      <c r="G20" s="42"/>
+      <c r="G20" s="46"/>
       <c r="H20" s="24"/>
     </row>
     <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -1590,7 +1593,7 @@
       <c r="F21" s="39">
         <v>5</v>
       </c>
-      <c r="G21" s="42"/>
+      <c r="G21" s="46"/>
       <c r="H21" s="24"/>
     </row>
     <row r="22" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1612,7 +1615,7 @@
       <c r="F22" s="39">
         <v>5</v>
       </c>
-      <c r="G22" s="42">
+      <c r="G22" s="46">
         <v>0</v>
       </c>
       <c r="H22" s="24"/>
@@ -1637,7 +1640,7 @@
         <f>IF($E23="Critical", 10, IF($E23="High",5, IF($E23="Low",1,"")))</f>
         <v>10</v>
       </c>
-      <c r="G23" s="42"/>
+      <c r="G23" s="46"/>
       <c r="H23" s="37" t="s">
         <v>23</v>
       </c>
@@ -1661,7 +1664,7 @@
       <c r="F24" s="39">
         <v>1</v>
       </c>
-      <c r="G24" s="42">
+      <c r="G24" s="46">
         <v>0</v>
       </c>
     </row>
@@ -1684,7 +1687,7 @@
       <c r="F25" s="39">
         <v>5</v>
       </c>
-      <c r="G25" s="42"/>
+      <c r="G25" s="46"/>
     </row>
     <row r="26" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
@@ -1705,7 +1708,7 @@
       <c r="F26" s="39">
         <v>1</v>
       </c>
-      <c r="G26" s="42"/>
+      <c r="G26" s="46"/>
     </row>
     <row r="27" spans="1:8" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A27" s="20">
@@ -1726,7 +1729,7 @@
       <c r="F27" s="39">
         <v>5</v>
       </c>
-      <c r="G27" s="42"/>
+      <c r="G27" s="46"/>
       <c r="H27" s="37" t="s">
         <v>23</v>
       </c>
@@ -1881,10 +1884,21 @@
       <c r="A35" s="20">
         <v>34</v>
       </c>
-      <c r="B35" s="26"/>
-      <c r="F35" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B35" s="26">
+        <v>2</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" s="39">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
@@ -6752,8 +6766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6770,16 +6784,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -7374,7 +7388,7 @@
       <c r="B23" s="9">
         <v>2</v>
       </c>
-      <c r="C23" s="45" t="s">
+      <c r="C23" s="41" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="17" t="s">
@@ -7400,10 +7414,10 @@
       <c r="B24" s="9">
         <v>2</v>
       </c>
-      <c r="C24" s="47" t="s">
+      <c r="C24" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="48" t="s">
+      <c r="D24" s="44" t="s">
         <v>64</v>
       </c>
       <c r="E24" s="38" t="s">
@@ -7427,7 +7441,7 @@
       <c r="B25" s="39">
         <v>2</v>
       </c>
-      <c r="C25" s="46" t="s">
+      <c r="C25" s="42" t="s">
         <v>66</v>
       </c>
       <c r="D25" s="24" t="s">
@@ -7450,7 +7464,7 @@
       <c r="B26" s="39">
         <v>2</v>
       </c>
-      <c r="C26" s="46" t="s">
+      <c r="C26" s="42" t="s">
         <v>66</v>
       </c>
       <c r="D26" s="24" t="s">
@@ -7473,7 +7487,7 @@
       <c r="B27" s="9">
         <v>2</v>
       </c>
-      <c r="C27" s="45" t="s">
+      <c r="C27" s="41" t="s">
         <v>66</v>
       </c>
       <c r="D27" s="17" t="s">
@@ -7496,7 +7510,7 @@
       <c r="B28" s="9">
         <v>2</v>
       </c>
-      <c r="C28" s="45" t="s">
+      <c r="C28" s="41" t="s">
         <v>56</v>
       </c>
       <c r="D28" s="17" t="s">
@@ -7518,7 +7532,7 @@
       <c r="B29" s="9">
         <v>2</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="41" t="s">
         <v>56</v>
       </c>
       <c r="D29" s="17" t="s">
@@ -7540,7 +7554,7 @@
       <c r="B30" s="9">
         <v>2</v>
       </c>
-      <c r="C30" s="45" t="s">
+      <c r="C30" s="41" t="s">
         <v>74</v>
       </c>
       <c r="D30" s="40" t="s">
@@ -7566,7 +7580,7 @@
       <c r="B31" s="9">
         <v>2</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="41" t="s">
         <v>42</v>
       </c>
       <c r="D31" s="15" t="s">
@@ -7592,7 +7606,7 @@
       <c r="B32" s="9">
         <v>2</v>
       </c>
-      <c r="C32" s="45" t="s">
+      <c r="C32" s="41" t="s">
         <v>56</v>
       </c>
       <c r="D32" s="17" t="s">
@@ -7614,7 +7628,7 @@
       <c r="B33" s="9">
         <v>2</v>
       </c>
-      <c r="C33" s="45" t="s">
+      <c r="C33" s="41" t="s">
         <v>56</v>
       </c>
       <c r="D33" s="10" t="s">
@@ -7629,13 +7643,25 @@
       <c r="G33" s="14"/>
       <c r="H33" s="13"/>
     </row>
-    <row r="34" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="14"/>
+    <row r="34" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>32</v>
+      </c>
+      <c r="B34" s="26">
+        <v>2</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="19">
+        <v>43754</v>
+      </c>
       <c r="G34" s="14"/>
       <c r="H34" s="13"/>
     </row>

</xml_diff>

<commit_message>
Resolved all current update bid bugs
For valid amount(amount<10 or >999) and if show invalid amount error if the input is non numerical

Co-Authored-By: bxtsang <bxtsang@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CasperLim\Documents\GitHub\project-g4t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4D24DB-DAFC-4C1B-9268-CE71C98E8143}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4F3D5B-E9C5-4C13-A114-1FCD86745E23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="81">
   <si>
     <t>Bug Log</t>
   </si>
@@ -6778,7 +6778,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7528,13 +7528,17 @@
         <v>71</v>
       </c>
       <c r="E28" s="38" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="F28" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="13"/>
+      <c r="G28" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="9">
@@ -7550,13 +7554,17 @@
         <v>72</v>
       </c>
       <c r="E29" s="38" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="F29" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G29" s="14"/>
-      <c r="H29" s="13"/>
+      <c r="G29" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="29" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
@@ -7624,13 +7632,17 @@
         <v>77</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="F32" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="13"/>
+      <c r="G32" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="9">

</xml_diff>

<commit_message>
Fixed bug for bidding
Display our own error when the post identifier is empty/alphabet

Co-Authored-By: bxtsang <bxtsang@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CasperLim\Documents\GitHub\project-g4t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4F3D5B-E9C5-4C13-A114-1FCD86745E23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889EBBD8-E1F7-4768-A5D6-57F4EB770A42}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="81">
   <si>
     <t>Bug Log</t>
   </si>
@@ -6778,7 +6778,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7482,13 +7482,17 @@
         <v>68</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="F26" s="14">
         <v>43749</v>
       </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="13"/>
+      <c r="G26" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="9">

</xml_diff>

<commit_message>
Debugging update bid amount bug
Update bid bug resolved. Updated bugmetric

Co-Authored-By: triciatll <triciatll@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CasperLim\Documents\GitHub\project-g4t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5B3809-6A24-436F-AD3F-602D62C3599B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05450189-7B4D-4685-8861-35D5956CD892}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="93">
   <si>
     <t>Bug Log</t>
   </si>
@@ -297,6 +297,18 @@
   </si>
   <si>
     <t>Round 2 update bid status is affected by other bids if there is multiple update at once</t>
+  </si>
+  <si>
+    <t>Timetable clashes when it is not suppose to clash</t>
+  </si>
+  <si>
+    <t>Bootstrap edollar validation displayed insufficient edollar despite have enough money</t>
+  </si>
+  <si>
+    <t>Exam and Class Timetable clashes when it is not suppose to clash</t>
+  </si>
+  <si>
+    <t>Minimum bid is wrong when the number of successful bid is equal to the number of vacancy</t>
   </si>
 </sst>
 </file>
@@ -593,7 +605,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none"/>
@@ -1184,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H999"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2030,6 +2126,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="G37" s="46">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="20">
@@ -2050,6 +2149,7 @@
       <c r="F38" s="39">
         <v>5</v>
       </c>
+      <c r="G38" s="46"/>
     </row>
     <row r="39" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="20">
@@ -2071,35 +2171,69 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="G39" s="46"/>
     </row>
     <row r="40" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A40" s="20">
         <v>39</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="F40" s="39" t="str">
+      <c r="B40" s="26">
+        <v>4</v>
+      </c>
+      <c r="C40" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" s="39">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="20">
         <v>40</v>
       </c>
-      <c r="B41" s="26"/>
-      <c r="F41" s="39" t="str">
+      <c r="B41" s="26">
+        <v>4</v>
+      </c>
+      <c r="C41" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E41" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" s="39">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="20">
         <v>41</v>
       </c>
-      <c r="B42" s="26"/>
-      <c r="F42" s="39" t="str">
+      <c r="B42" s="26">
+        <v>4</v>
+      </c>
+      <c r="C42" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E42" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" s="39">
         <f t="shared" si="0"/>
-        <v/>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
@@ -6873,7 +7007,8 @@
       <c r="B999" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="G37:G39"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="G3:G21"/>
     <mergeCell ref="G22:G23"/>
@@ -6881,7 +7016,7 @@
     <mergeCell ref="G28:G36"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="39" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6898,8 +7033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7843,13 +7978,17 @@
         <v>80</v>
       </c>
       <c r="E35" s="38" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="F35" s="19">
         <v>43754</v>
       </c>
-      <c r="G35" s="14"/>
-      <c r="H35" s="13"/>
+      <c r="G35" s="19">
+        <v>43774</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="36" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
@@ -7887,13 +8026,17 @@
         <v>80</v>
       </c>
       <c r="E37" s="38" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="F37" s="19">
         <v>43754</v>
       </c>
-      <c r="G37" s="14"/>
-      <c r="H37" s="13"/>
+      <c r="G37" s="19">
+        <v>43774</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="38" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
@@ -7909,7 +8052,7 @@
         <v>83</v>
       </c>
       <c r="E38" s="38" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="F38" s="19" t="s">
         <v>84</v>
@@ -7974,34 +8117,78 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="13"/>
-    </row>
-    <row r="42" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="14"/>
+      <c r="A41" s="9">
+        <v>39</v>
+      </c>
+      <c r="B41" s="9">
+        <v>4</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="19">
+        <v>43774</v>
+      </c>
+      <c r="G41" s="19">
+        <v>43774</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="9">
+        <v>40</v>
+      </c>
+      <c r="B42" s="9">
+        <v>4</v>
+      </c>
+      <c r="C42" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E42" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42" s="19">
+        <v>43774</v>
+      </c>
       <c r="G42" s="14"/>
       <c r="H42" s="13"/>
     </row>
-    <row r="43" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="13"/>
+    <row r="43" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="9">
+        <v>41</v>
+      </c>
+      <c r="B43" s="9">
+        <v>4</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="19">
+        <v>43774</v>
+      </c>
+      <c r="G43" s="19">
+        <v>43774</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="44" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="9"/>
@@ -17578,142 +17765,187 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="43" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="cellIs" dxfId="25" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="44" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="containsBlanks" dxfId="24" priority="36">
+    <cfRule type="containsBlanks" dxfId="36" priority="45">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E30 E33:E38">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="31" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E30 E33:E38">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E30 E33:E38">
-    <cfRule type="containsBlanks" dxfId="21" priority="24">
+    <cfRule type="containsBlanks" dxfId="33" priority="33">
       <formula>LEN(TRIM(E23))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsBlanks" dxfId="18" priority="21">
+    <cfRule type="containsBlanks" dxfId="30" priority="30">
       <formula>LEN(TRIM(E12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="containsBlanks" dxfId="15" priority="18">
+    <cfRule type="containsBlanks" dxfId="27" priority="27">
       <formula>LEN(TRIM(E21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="containsBlanks" dxfId="12" priority="15">
+    <cfRule type="containsBlanks" dxfId="24" priority="24">
       <formula>LEN(TRIM(E22))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsBlanks" dxfId="9" priority="12">
+    <cfRule type="containsBlanks" dxfId="21" priority="21">
       <formula>LEN(TRIM(E31))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="containsBlanks" dxfId="18" priority="18">
+      <formula>LEN(TRIM(E32))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="containsBlanks" dxfId="15" priority="15">
+      <formula>LEN(TRIM(E39))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="containsBlanks" dxfId="12" priority="12">
+      <formula>LEN(TRIM(E40))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E41">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E41">
     <cfRule type="containsBlanks" dxfId="6" priority="9">
-      <formula>LEN(TRIM(E32))=0</formula>
+      <formula>LEN(TRIM(E41))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
+  <conditionalFormatting sqref="E42">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
+  <conditionalFormatting sqref="E42">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
+  <conditionalFormatting sqref="E42">
     <cfRule type="containsBlanks" dxfId="3" priority="6">
-      <formula>LEN(TRIM(E39))=0</formula>
+      <formula>LEN(TRIM(E42))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
+  <conditionalFormatting sqref="E43">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
+  <conditionalFormatting sqref="E43">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
+  <conditionalFormatting sqref="E43">
     <cfRule type="containsBlanks" dxfId="0" priority="3">
-      <formula>LEN(TRIM(E40))=0</formula>
+      <formula>LEN(TRIM(E43))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E3:E40" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="E3:E43" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Unresolved,Resolved"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Debugged for end of round error
When the round is completed, we will tell them so and do not allow them to choose the mods.

Co-Authored-By: yan-ning <yan-ning@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CasperLim\Documents\GitHub\project-g4t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FF8AED-24DF-43AD-8EFD-1C37D41979BF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB68BA8-CAD0-4C6A-BBB6-DCD5C24AA1B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="98">
   <si>
     <t>Bug Log</t>
   </si>
@@ -629,49 +629,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="46">
     <dxf>
       <fill>
         <patternFill patternType="none"/>
@@ -1388,7 +1346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
@@ -7157,7 +7115,7 @@
     <mergeCell ref="G28:G36"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="51" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="45" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7174,8 +7132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8345,13 +8303,17 @@
         <v>93</v>
       </c>
       <c r="E44" s="38" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="F44" s="19">
         <v>43776</v>
       </c>
-      <c r="G44" s="14"/>
-      <c r="H44" s="13"/>
+      <c r="G44" s="14">
+        <v>43783</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="45" spans="1:8" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A45" s="46">
@@ -17950,212 +17912,212 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="53" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="containsBlanks" dxfId="48" priority="54">
+    <cfRule type="containsBlanks" dxfId="42" priority="54">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E30 E33:E38">
-    <cfRule type="cellIs" dxfId="47" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E30 E33:E38">
-    <cfRule type="cellIs" dxfId="46" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E30 E33:E38">
-    <cfRule type="containsBlanks" dxfId="45" priority="42">
+    <cfRule type="containsBlanks" dxfId="39" priority="42">
       <formula>LEN(TRIM(E23))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="44" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="43" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsBlanks" dxfId="42" priority="39">
+    <cfRule type="containsBlanks" dxfId="36" priority="39">
       <formula>LEN(TRIM(E12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="41" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="40" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="containsBlanks" dxfId="39" priority="36">
+    <cfRule type="containsBlanks" dxfId="33" priority="36">
       <formula>LEN(TRIM(E21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="38" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="37" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="containsBlanks" dxfId="36" priority="33">
+    <cfRule type="containsBlanks" dxfId="30" priority="33">
       <formula>LEN(TRIM(E22))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="35" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="34" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsBlanks" dxfId="33" priority="30">
+    <cfRule type="containsBlanks" dxfId="27" priority="30">
       <formula>LEN(TRIM(E31))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="32" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="31" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="containsBlanks" dxfId="30" priority="27">
+    <cfRule type="containsBlanks" dxfId="24" priority="27">
       <formula>LEN(TRIM(E32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="29" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="28" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="containsBlanks" dxfId="27" priority="24">
+    <cfRule type="containsBlanks" dxfId="21" priority="24">
       <formula>LEN(TRIM(E39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="25" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsBlanks" dxfId="24" priority="21">
+    <cfRule type="containsBlanks" dxfId="18" priority="21">
       <formula>LEN(TRIM(E40))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" dxfId="23" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" dxfId="22" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsBlanks" dxfId="21" priority="18">
+    <cfRule type="containsBlanks" dxfId="15" priority="18">
       <formula>LEN(TRIM(E41))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="containsBlanks" dxfId="18" priority="15">
+    <cfRule type="containsBlanks" dxfId="12" priority="15">
       <formula>LEN(TRIM(E42))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="containsBlanks" dxfId="15" priority="12">
+    <cfRule type="containsBlanks" dxfId="9" priority="12">
       <formula>LEN(TRIM(E43))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="containsBlanks" dxfId="12" priority="9">
+    <cfRule type="containsBlanks" dxfId="6" priority="9">
       <formula>LEN(TRIM(E44))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="containsBlanks" dxfId="9" priority="6">
+    <cfRule type="containsBlanks" dxfId="3" priority="6">
       <formula>LEN(TRIM(E45))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Bugs found when testing
Bugs found:
1. Number of vacancy not updated in db when section is dropped
2. Incorrect timezone in admin page
3. S/N of updated bids should start from 1 instead
4. Duplicate "go back to home" link
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ong Yan Ning\Documents\GitHub\project-g4t4\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Spm project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AD1E42-6ACE-4379-B65A-D8808B6899F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB08D012-1F71-444A-85C3-46520C601DD2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="112">
   <si>
     <t>Bug Log</t>
   </si>
@@ -352,6 +352,21 @@
   <si>
     <t>Unresolved</t>
   </si>
+  <si>
+    <t>Number of vacancy in database not reflected accordinly upon dropping section during round 2</t>
+  </si>
+  <si>
+    <t>2 "go back to home" link upon clicking "update bid" in round 2</t>
+  </si>
+  <si>
+    <t>Timezone in admin interface not accurate (eg. should be 17 November 2019 instead of 16 November 2019) in midnight</t>
+  </si>
+  <si>
+    <t>Update bid</t>
+  </si>
+  <si>
+    <t>S/N should start with 1 instead of 0 upon updating bid</t>
+  </si>
 </sst>
 </file>
 
@@ -503,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -657,6 +672,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -668,7 +686,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="70">
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none"/>
@@ -1532,8 +1571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1550,16 +1589,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -1607,7 +1646,7 @@
         <f t="shared" ref="F3:F199" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G3" s="52">
+      <c r="G3" s="53">
         <v>0</v>
       </c>
       <c r="H3" s="24" t="str">
@@ -1635,7 +1674,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="53"/>
       <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1658,7 +1697,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="53"/>
       <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -1681,7 +1720,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G6" s="52"/>
+      <c r="G6" s="53"/>
       <c r="H6" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1704,7 +1743,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G7" s="52"/>
+      <c r="G7" s="53"/>
       <c r="H7" s="24"/>
     </row>
     <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1727,7 +1766,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G8" s="52"/>
+      <c r="G8" s="53"/>
       <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1750,7 +1789,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G9" s="52"/>
+      <c r="G9" s="53"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1773,7 +1812,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G10" s="52"/>
+      <c r="G10" s="53"/>
       <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1796,7 +1835,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G11" s="52"/>
+      <c r="G11" s="53"/>
       <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1819,7 +1858,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G12" s="52"/>
+      <c r="G12" s="53"/>
       <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1842,7 +1881,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G13" s="52"/>
+      <c r="G13" s="53"/>
       <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1864,7 +1903,7 @@
       <c r="F14" s="39">
         <v>1</v>
       </c>
-      <c r="G14" s="52"/>
+      <c r="G14" s="53"/>
       <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1886,7 +1925,7 @@
       <c r="F15" s="39">
         <v>5</v>
       </c>
-      <c r="G15" s="52"/>
+      <c r="G15" s="53"/>
       <c r="H15" s="24"/>
     </row>
     <row r="16" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1908,7 +1947,7 @@
       <c r="F16" s="39">
         <v>1</v>
       </c>
-      <c r="G16" s="52"/>
+      <c r="G16" s="53"/>
       <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1930,7 +1969,7 @@
       <c r="F17" s="39">
         <v>5</v>
       </c>
-      <c r="G17" s="52"/>
+      <c r="G17" s="53"/>
       <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1952,7 +1991,7 @@
       <c r="F18" s="39">
         <v>5</v>
       </c>
-      <c r="G18" s="52"/>
+      <c r="G18" s="53"/>
       <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1974,7 +2013,7 @@
       <c r="F19" s="39">
         <v>10</v>
       </c>
-      <c r="G19" s="52"/>
+      <c r="G19" s="53"/>
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1996,7 +2035,7 @@
       <c r="F20" s="39">
         <v>5</v>
       </c>
-      <c r="G20" s="52"/>
+      <c r="G20" s="53"/>
       <c r="H20" s="24"/>
     </row>
     <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
@@ -2018,7 +2057,7 @@
       <c r="F21" s="39">
         <v>5</v>
       </c>
-      <c r="G21" s="52"/>
+      <c r="G21" s="53"/>
       <c r="H21" s="24"/>
     </row>
     <row r="22" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -2040,7 +2079,7 @@
       <c r="F22" s="39">
         <v>5</v>
       </c>
-      <c r="G22" s="52">
+      <c r="G22" s="53">
         <v>0</v>
       </c>
       <c r="H22" s="24"/>
@@ -2065,7 +2104,7 @@
         <f>IF($E23="Critical", 10, IF($E23="High",5, IF($E23="Low",1,"")))</f>
         <v>10</v>
       </c>
-      <c r="G23" s="52"/>
+      <c r="G23" s="53"/>
       <c r="H23" s="37" t="s">
         <v>23</v>
       </c>
@@ -2089,7 +2128,7 @@
       <c r="F24" s="39">
         <v>1</v>
       </c>
-      <c r="G24" s="52">
+      <c r="G24" s="53">
         <v>0</v>
       </c>
     </row>
@@ -2112,7 +2151,7 @@
       <c r="F25" s="39">
         <v>5</v>
       </c>
-      <c r="G25" s="52"/>
+      <c r="G25" s="53"/>
     </row>
     <row r="26" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
@@ -2133,7 +2172,7 @@
       <c r="F26" s="39">
         <v>1</v>
       </c>
-      <c r="G26" s="52"/>
+      <c r="G26" s="53"/>
     </row>
     <row r="27" spans="1:8" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A27" s="20">
@@ -2154,7 +2193,7 @@
       <c r="F27" s="39">
         <v>5</v>
       </c>
-      <c r="G27" s="52"/>
+      <c r="G27" s="53"/>
       <c r="H27" s="37" t="s">
         <v>23</v>
       </c>
@@ -2178,7 +2217,7 @@
       <c r="F28" s="39">
         <v>1</v>
       </c>
-      <c r="G28" s="52">
+      <c r="G28" s="53">
         <v>0</v>
       </c>
     </row>
@@ -2202,7 +2241,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G29" s="52"/>
+      <c r="G29" s="53"/>
     </row>
     <row r="30" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="20">
@@ -2224,7 +2263,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G30" s="52"/>
+      <c r="G30" s="53"/>
     </row>
     <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
@@ -2246,7 +2285,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G31" s="52"/>
+      <c r="G31" s="53"/>
     </row>
     <row r="32" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="20">
@@ -2268,7 +2307,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G32" s="52"/>
+      <c r="G32" s="53"/>
     </row>
     <row r="33" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="20">
@@ -2290,7 +2329,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G33" s="52"/>
+      <c r="G33" s="53"/>
     </row>
     <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A34" s="20">
@@ -2312,7 +2351,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G34" s="52"/>
+      <c r="G34" s="53"/>
     </row>
     <row r="35" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A35" s="20">
@@ -2334,7 +2373,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G35" s="52"/>
+      <c r="G35" s="53"/>
     </row>
     <row r="36" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
@@ -2356,7 +2395,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G36" s="52"/>
+      <c r="G36" s="53"/>
     </row>
     <row r="37" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
@@ -2378,7 +2417,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G37" s="52">
+      <c r="G37" s="53">
         <v>0</v>
       </c>
     </row>
@@ -2401,7 +2440,7 @@
       <c r="F38" s="39">
         <v>5</v>
       </c>
-      <c r="G38" s="52"/>
+      <c r="G38" s="53"/>
     </row>
     <row r="39" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="20">
@@ -2423,7 +2462,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G39" s="52"/>
+      <c r="G39" s="53"/>
     </row>
     <row r="40" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A40" s="20">
@@ -2698,44 +2737,88 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A53" s="20">
         <v>52</v>
       </c>
-      <c r="B53" s="26"/>
-      <c r="F53" s="39" t="str">
+      <c r="B53" s="26">
+        <v>4</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D53" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E53" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="F53" s="52">
         <f t="shared" si="0"/>
-        <v/>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A54" s="20">
         <v>53</v>
       </c>
-      <c r="B54" s="26"/>
-      <c r="F54" s="39" t="str">
+      <c r="B54" s="26">
+        <v>4</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="E54" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="F54" s="52">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A55" s="20">
         <v>54</v>
       </c>
-      <c r="B55" s="26"/>
-      <c r="F55" s="39" t="str">
+      <c r="B55" s="26">
+        <v>4</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E55" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="F55" s="52">
         <f t="shared" si="0"/>
-        <v/>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A56" s="20">
         <v>55</v>
       </c>
-      <c r="B56" s="26"/>
-      <c r="F56" s="39" t="str">
+      <c r="B56" s="26">
+        <v>4</v>
+      </c>
+      <c r="C56" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D56" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="E56" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" s="52">
         <f t="shared" si="0"/>
-        <v/>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
@@ -7378,7 +7461,7 @@
     <mergeCell ref="G28:G36"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="66" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="69" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7396,7 +7479,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView topLeftCell="A42" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7413,16 +7496,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
     </row>
     <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -8816,43 +8899,91 @@
       <c r="G53" s="14"/>
       <c r="H53" s="13"/>
     </row>
-    <row r="54" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="14"/>
+    <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A54" s="9">
+        <v>52</v>
+      </c>
+      <c r="B54" s="26">
+        <v>4</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="F54" s="14">
+        <v>43786</v>
+      </c>
       <c r="G54" s="14"/>
       <c r="H54" s="13"/>
     </row>
-    <row r="55" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A55" s="9"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="14"/>
+    <row r="55" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9">
+        <v>53</v>
+      </c>
+      <c r="B55" s="26">
+        <v>4</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="E55" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="F55" s="14">
+        <v>43786</v>
+      </c>
       <c r="G55" s="14"/>
       <c r="H55" s="13"/>
     </row>
-    <row r="56" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="14"/>
+    <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A56" s="9">
+        <v>54</v>
+      </c>
+      <c r="B56" s="26">
+        <v>4</v>
+      </c>
+      <c r="C56" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="F56" s="14">
+        <v>43786</v>
+      </c>
       <c r="G56" s="14"/>
       <c r="H56" s="13"/>
     </row>
-    <row r="57" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A57" s="9"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="14"/>
+    <row r="57" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A57" s="9">
+        <v>55</v>
+      </c>
+      <c r="B57" s="26">
+        <v>4</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="E57" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="F57" s="14">
+        <v>43786</v>
+      </c>
       <c r="G57" s="14"/>
       <c r="H57" s="13"/>
     </row>
@@ -18291,337 +18422,352 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="cellIs" dxfId="65" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="76" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="cellIs" dxfId="64" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="77" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="containsBlanks" dxfId="63" priority="75">
+    <cfRule type="containsBlanks" dxfId="66" priority="78">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E30 E33:E38">
+    <cfRule type="cellIs" dxfId="65" priority="64" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23:E30 E33:E38">
+    <cfRule type="cellIs" dxfId="64" priority="65" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23:E30 E33:E38">
+    <cfRule type="containsBlanks" dxfId="63" priority="66">
+      <formula>LEN(TRIM(E23))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
     <cfRule type="cellIs" dxfId="62" priority="61" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23:E30 E33:E38">
+  <conditionalFormatting sqref="E12">
     <cfRule type="cellIs" dxfId="61" priority="62" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23:E30 E33:E38">
+  <conditionalFormatting sqref="E12">
     <cfRule type="containsBlanks" dxfId="60" priority="63">
-      <formula>LEN(TRIM(E23))=0</formula>
+      <formula>LEN(TRIM(E12))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
+  <conditionalFormatting sqref="E21">
     <cfRule type="cellIs" dxfId="59" priority="58" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
+  <conditionalFormatting sqref="E21">
     <cfRule type="cellIs" dxfId="58" priority="59" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
+  <conditionalFormatting sqref="E21">
     <cfRule type="containsBlanks" dxfId="57" priority="60">
-      <formula>LEN(TRIM(E12))=0</formula>
+      <formula>LEN(TRIM(E21))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="E22">
     <cfRule type="cellIs" dxfId="56" priority="55" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="E22">
     <cfRule type="cellIs" dxfId="55" priority="56" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="E22">
     <cfRule type="containsBlanks" dxfId="54" priority="57">
-      <formula>LEN(TRIM(E21))=0</formula>
+      <formula>LEN(TRIM(E22))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
+  <conditionalFormatting sqref="E31">
     <cfRule type="cellIs" dxfId="53" priority="52" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
+  <conditionalFormatting sqref="E31">
     <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
+  <conditionalFormatting sqref="E31">
     <cfRule type="containsBlanks" dxfId="51" priority="54">
-      <formula>LEN(TRIM(E22))=0</formula>
+      <formula>LEN(TRIM(E31))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
+  <conditionalFormatting sqref="E32">
     <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
+  <conditionalFormatting sqref="E32">
     <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
+  <conditionalFormatting sqref="E32">
     <cfRule type="containsBlanks" dxfId="48" priority="51">
-      <formula>LEN(TRIM(E31))=0</formula>
+      <formula>LEN(TRIM(E32))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E39">
     <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E39">
     <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E39">
     <cfRule type="containsBlanks" dxfId="45" priority="48">
-      <formula>LEN(TRIM(E32))=0</formula>
+      <formula>LEN(TRIM(E39))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
+  <conditionalFormatting sqref="E40">
     <cfRule type="cellIs" dxfId="44" priority="43" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
+  <conditionalFormatting sqref="E40">
     <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
+  <conditionalFormatting sqref="E40">
     <cfRule type="containsBlanks" dxfId="42" priority="45">
-      <formula>LEN(TRIM(E39))=0</formula>
+      <formula>LEN(TRIM(E40))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
+  <conditionalFormatting sqref="E41">
     <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
+  <conditionalFormatting sqref="E41">
     <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
+  <conditionalFormatting sqref="E41">
     <cfRule type="containsBlanks" dxfId="39" priority="42">
-      <formula>LEN(TRIM(E40))=0</formula>
+      <formula>LEN(TRIM(E41))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
+  <conditionalFormatting sqref="E42">
     <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
+  <conditionalFormatting sqref="E42">
     <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
+  <conditionalFormatting sqref="E42">
     <cfRule type="containsBlanks" dxfId="36" priority="39">
-      <formula>LEN(TRIM(E41))=0</formula>
+      <formula>LEN(TRIM(E42))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
+  <conditionalFormatting sqref="E43">
     <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
+  <conditionalFormatting sqref="E43">
     <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
+  <conditionalFormatting sqref="E43">
     <cfRule type="containsBlanks" dxfId="33" priority="36">
-      <formula>LEN(TRIM(E42))=0</formula>
+      <formula>LEN(TRIM(E43))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
+  <conditionalFormatting sqref="E44">
     <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
+  <conditionalFormatting sqref="E44">
     <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
+  <conditionalFormatting sqref="E44">
     <cfRule type="containsBlanks" dxfId="30" priority="33">
-      <formula>LEN(TRIM(E43))=0</formula>
+      <formula>LEN(TRIM(E44))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
+  <conditionalFormatting sqref="E45">
     <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
+  <conditionalFormatting sqref="E45">
     <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
+  <conditionalFormatting sqref="E45">
     <cfRule type="containsBlanks" dxfId="27" priority="30">
-      <formula>LEN(TRIM(E44))=0</formula>
+      <formula>LEN(TRIM(E45))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
+  <conditionalFormatting sqref="E46">
     <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
+  <conditionalFormatting sqref="E46">
     <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
+  <conditionalFormatting sqref="E46">
     <cfRule type="containsBlanks" dxfId="24" priority="27">
-      <formula>LEN(TRIM(E45))=0</formula>
+      <formula>LEN(TRIM(E46))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
+  <conditionalFormatting sqref="E47">
     <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
+  <conditionalFormatting sqref="E47">
     <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
+  <conditionalFormatting sqref="E47">
     <cfRule type="containsBlanks" dxfId="21" priority="24">
-      <formula>LEN(TRIM(E46))=0</formula>
+      <formula>LEN(TRIM(E47))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E47">
+  <conditionalFormatting sqref="E48">
     <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E47">
+  <conditionalFormatting sqref="E48">
     <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E47">
+  <conditionalFormatting sqref="E48">
     <cfRule type="containsBlanks" dxfId="18" priority="21">
-      <formula>LEN(TRIM(E47))=0</formula>
+      <formula>LEN(TRIM(E48))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
+  <conditionalFormatting sqref="E49">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
+  <conditionalFormatting sqref="E49">
     <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
+  <conditionalFormatting sqref="E49">
     <cfRule type="containsBlanks" dxfId="15" priority="18">
-      <formula>LEN(TRIM(E48))=0</formula>
+      <formula>LEN(TRIM(E49))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49">
+  <conditionalFormatting sqref="E50">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49">
+  <conditionalFormatting sqref="E50">
     <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49">
+  <conditionalFormatting sqref="E50">
     <cfRule type="containsBlanks" dxfId="12" priority="15">
-      <formula>LEN(TRIM(E49))=0</formula>
+      <formula>LEN(TRIM(E50))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50">
+  <conditionalFormatting sqref="E51">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50">
+  <conditionalFormatting sqref="E51">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50">
+  <conditionalFormatting sqref="E51">
     <cfRule type="containsBlanks" dxfId="9" priority="12">
-      <formula>LEN(TRIM(E50))=0</formula>
+      <formula>LEN(TRIM(E51))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
+  <conditionalFormatting sqref="E52">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
+  <conditionalFormatting sqref="E52">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
+  <conditionalFormatting sqref="E52">
     <cfRule type="containsBlanks" dxfId="6" priority="9">
-      <formula>LEN(TRIM(E51))=0</formula>
+      <formula>LEN(TRIM(E52))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
+  <conditionalFormatting sqref="E53">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
+  <conditionalFormatting sqref="E53">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
+  <conditionalFormatting sqref="E53">
     <cfRule type="containsBlanks" dxfId="3" priority="6">
-      <formula>LEN(TRIM(E52))=0</formula>
+      <formula>LEN(TRIM(E53))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
+  <conditionalFormatting sqref="E54:E57">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
+  <conditionalFormatting sqref="E54:E57">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
+  <conditionalFormatting sqref="E54:E57">
     <cfRule type="containsBlanks" dxfId="0" priority="3">
-      <formula>LEN(TRIM(E53))=0</formula>
+      <formula>LEN(TRIM(E54))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E3:E53" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="E3:E57" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Unresolved,Resolved"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated manual testing and bugs metric
Updated manual testing and bugs solved
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Spm project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ong Yan Ning\Documents\GitHub\project-g4t4\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB08D012-1F71-444A-85C3-46520C601DD2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F127249-37D8-4784-9879-C56B04595C4E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="112">
   <si>
     <t>Bug Log</t>
   </si>
@@ -7478,8 +7478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="A45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8935,13 +8935,17 @@
         <v>108</v>
       </c>
       <c r="E55" s="38" t="s">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="F55" s="14">
         <v>43786</v>
       </c>
-      <c r="G55" s="14"/>
-      <c r="H55" s="13"/>
+      <c r="G55" s="14">
+        <v>43786</v>
+      </c>
+      <c r="H55" s="18" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
@@ -8957,13 +8961,17 @@
         <v>109</v>
       </c>
       <c r="E56" s="38" t="s">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="F56" s="14">
         <v>43786</v>
       </c>
-      <c r="G56" s="14"/>
-      <c r="H56" s="13"/>
+      <c r="G56" s="14">
+        <v>43786</v>
+      </c>
+      <c r="H56" s="18" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="57" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A57" s="9">

</xml_diff>